<commit_message>
Updated burndown chart name
</commit_message>
<xml_diff>
--- a/SprintTaskSheet.xlsx
+++ b/SprintTaskSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prkarve/Documents/cmpe-202/team-hackathon/fa19-202-firebirds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08968B7-98D9-6444-822B-37B15E862BD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5BEA57-BECA-D343-8032-9D9EFB55B852}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint" sheetId="1" r:id="rId1"/>
@@ -869,7 +869,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Burndown (Team XXX)</a:t>
+              <a:t>Burndown (Team Firebirds)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1626,7 +1626,7 @@
   </sheetPr>
   <dimension ref="A1:Q999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
+    <sheetView zoomScale="142" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -18290,7 +18290,9 @@
   </sheetPr>
   <dimension ref="A1:Z986"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>

</xml_diff>